<commit_message>
Add Member_Daily_Report version 2
</commit_message>
<xml_diff>
--- a/Member_Daily_Report.xlsx
+++ b/Member_Daily_Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT Soft Learning\IT_Java_FullStack\JWD\Assignment\MockProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81382C07-BADC-4C4D-AC12-29B076E09D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FA93C0-2067-4FD0-9BBA-D1F92598E1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoang_Anh" sheetId="1" r:id="rId1"/>
@@ -241,9 +241,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -259,14 +256,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -284,6 +284,630 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>541020</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B50876F-A5BB-4E64-A6AD-2BAAD394EDDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5052060" y="1630680"/>
+          <a:ext cx="3741420" cy="525780"/>
+          <a:chOff x="3939540" y="1501140"/>
+          <a:chExt cx="3741420" cy="525780"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Arrow: Left 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E04164C1-9D98-A08A-16AD-D13382310ABF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3939540" y="1554480"/>
+            <a:ext cx="815340" cy="411480"/>
+          </a:xfrm>
+          <a:prstGeom prst="leftArrow">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48108D2F-A71A-5B16-69E7-19E21E65C148}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4846320" y="1501140"/>
+            <a:ext cx="2834640" cy="525780"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Điền</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> link trực tiếp file của mình trên github, ko phải link repository cả nhóm</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>533400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB501B1A-9CF6-4C54-8C99-53BD40C22B1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4145280" y="1318260"/>
+          <a:ext cx="3741420" cy="525780"/>
+          <a:chOff x="3939540" y="1501140"/>
+          <a:chExt cx="3741420" cy="525780"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Arrow: Left 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40183A3D-970A-A252-E265-9977F9EF4DF9}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3939540" y="1554480"/>
+            <a:ext cx="815340" cy="411480"/>
+          </a:xfrm>
+          <a:prstGeom prst="leftArrow">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{240D4C8A-AAFA-B6A0-ADF5-B2BD4A2A3DDB}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4846320" y="1501140"/>
+            <a:ext cx="2834640" cy="525780"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Điền</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> link trực tiếp file của mình trên github, ko phải link repository cả nhóm</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>541020</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC9CE528-563F-4E80-A453-5454D4631F88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3802380" y="1478280"/>
+          <a:ext cx="3741420" cy="525780"/>
+          <a:chOff x="3939540" y="1501140"/>
+          <a:chExt cx="3741420" cy="525780"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Arrow: Left 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E96AC9A7-EBFA-DBDE-AFBC-35DB7FFF0920}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3939540" y="1554480"/>
+            <a:ext cx="815340" cy="411480"/>
+          </a:xfrm>
+          <a:prstGeom prst="leftArrow">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Rectangle: Rounded Corners 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44D566CE-7247-DEE7-5B81-3911B85399DC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4846320" y="1501140"/>
+            <a:ext cx="2834640" cy="525780"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Điền</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> link trực tiếp file của mình trên github, ko phải link repository cả nhóm</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="4" name="Group 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0756A1E0-AC46-E489-70D3-3C54E1E769DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3939540" y="1501140"/>
+          <a:ext cx="3741420" cy="525780"/>
+          <a:chOff x="3939540" y="1501140"/>
+          <a:chExt cx="3741420" cy="525780"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="2" name="Arrow: Left 1">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{160B834D-546E-4C1C-1116-129A5583672A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3939540" y="1554480"/>
+            <a:ext cx="815340" cy="411480"/>
+          </a:xfrm>
+          <a:prstGeom prst="leftArrow">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Rectangle: Rounded Corners 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40D57FF9-BC65-B4B8-F80A-3791EB903AA4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4846320" y="1501140"/>
+            <a:ext cx="2834640" cy="525780"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Điền</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> link trực tiếp file của mình trên github, ko phải link repository cả nhóm</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,7 +1176,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,76 +1194,76 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -653,6 +1277,7 @@
     <hyperlink ref="B8" r:id="rId1" xr:uid="{97756743-B39A-450E-B510-1B6CEF7B4B64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -661,7 +1286,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,76 +1304,76 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -762,6 +1387,7 @@
     <hyperlink ref="B8" r:id="rId1" xr:uid="{972D23BF-FC7C-47CD-908F-E5D4DE485C8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -769,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDCA803-221C-4140-8582-859A985E5E0C}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,76 +1414,76 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -871,6 +1497,7 @@
     <hyperlink ref="B8" r:id="rId1" xr:uid="{D6E620C6-3210-4D99-86B7-960FD32F74DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -878,13 +1505,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79EBCF5B-D4B5-47BF-8D1E-DEED0C94919C}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" style="11" customWidth="1"/>
+    <col min="1" max="1" width="22" style="9" customWidth="1"/>
     <col min="2" max="2" width="34.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -897,78 +1524,78 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8" t="s">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11"/>
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
@@ -982,5 +1609,6 @@
     <hyperlink ref="B8" r:id="rId1" xr:uid="{1B4D6CF2-0AED-4BEC-B36C-6524D276BB65}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>